<commit_message>
refactor/ consistent naming; const maps replace all enums; linting
</commit_message>
<xml_diff>
--- a/lib/StockTake_24.xlsx
+++ b/lib/StockTake_24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conrad/Documents/portfolio/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9B6944-C432-5E4F-B06F-F63358E5DB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484E7AE5-96B1-7648-B8E5-53A0404426BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="1200" windowWidth="32160" windowHeight="25980" xr2:uid="{477BC4CC-D0A8-164E-A5E9-23EF0DA1317C}"/>
+    <workbookView xWindow="1240" yWindow="520" windowWidth="32160" windowHeight="23560" xr2:uid="{477BC4CC-D0A8-164E-A5E9-23EF0DA1317C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,6 +554,13 @@
       <color theme="1"/>
       <name val="Avenir Book"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -641,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,22 +666,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -693,16 +692,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -883,22 +872,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DFCA3A6-CA22-4847-8C93-F0109546E0B7}" name="Table1" displayName="Table1" ref="I1:O83" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DFCA3A6-CA22-4847-8C93-F0109546E0B7}" name="Table1" displayName="Table1" ref="I1:O83" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="I1:O83" xr:uid="{7DFCA3A6-CA22-4847-8C93-F0109546E0B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CA5743FA-4063-1244-90CD-07FA762C1AB3}" name="Material" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DD1AA96D-6FF1-DE46-807F-B4491BDF2C8A}" name="Exp-Virgin" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{CA5743FA-4063-1244-90CD-07FA762C1AB3}" name="Material" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DD1AA96D-6FF1-DE46-807F-B4491BDF2C8A}" name="Exp-Virgin" dataDxfId="7">
       <calculatedColumnFormula array="1">INDEX($D$1:$D$140, (ROW())*2-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7A95806F-5FDD-484A-8F4F-1FD4D83F3B5D}" name="Actual-Virgin" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{7A95806F-5FDD-484A-8F4F-1FD4D83F3B5D}" name="Actual-Virgin" dataDxfId="6">
       <calculatedColumnFormula array="1">INDEX($E$1:$E$140, (ROW())*2-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5EAE7938-45AB-6D41-909E-92B2FB40B97F}" name="Difference-V" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{5EAE7938-45AB-6D41-909E-92B2FB40B97F}" name="Difference-V" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[Actual-Virgin]]-Table1[[#This Row],[Exp-Virgin]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7B3CD012-5CAC-1F44-AC84-671FD53BD9A2}" name="Exp-Repro" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{568CA394-B911-9C44-A615-77CDC517BAB4}" name="Actual-Repro" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{CBA3DF0A-538B-FC47-9985-8D4993A4925B}" name="Difference-R" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{7B3CD012-5CAC-1F44-AC84-671FD53BD9A2}" name="Exp-Repro" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{568CA394-B911-9C44-A615-77CDC517BAB4}" name="Actual-Repro" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{CBA3DF0A-538B-FC47-9985-8D4993A4925B}" name="Difference-R" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[Actual-Repro]]-Table1[[#This Row],[Exp-Repro]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1226,7 +1215,7 @@
   <dimension ref="A1:W142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2975,7 +2964,7 @@
       <c r="J28" s="4">
         <v>0</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="2">
         <v>0</v>
       </c>
       <c r="L28" s="6">
@@ -2985,7 +2974,7 @@
       <c r="M28" s="4">
         <v>0</v>
       </c>
-      <c r="N28" s="11">
+      <c r="N28" s="2">
         <v>0</v>
       </c>
       <c r="O28" s="4">
@@ -3978,13 +3967,13 @@
       <c r="G45" s="1">
         <v>0</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="2" t="s">
         <v>59</v>
       </c>
       <c r="J45" s="4">
         <v>2</v>
       </c>
-      <c r="K45" s="11">
+      <c r="K45" s="2">
         <v>0</v>
       </c>
       <c r="L45" s="6">
@@ -3994,7 +3983,7 @@
       <c r="M45" s="4">
         <v>0</v>
       </c>
-      <c r="N45" s="11">
+      <c r="N45" s="2">
         <v>0</v>
       </c>
       <c r="O45" s="4">
@@ -4040,13 +4029,13 @@
       <c r="G46" s="1">
         <v>0</v>
       </c>
-      <c r="I46" s="11" t="s">
+      <c r="I46" s="2" t="s">
         <v>61</v>
       </c>
       <c r="J46" s="4">
         <v>0</v>
       </c>
-      <c r="K46" s="11">
+      <c r="K46" s="2">
         <v>1</v>
       </c>
       <c r="L46" s="6">
@@ -4056,7 +4045,7 @@
       <c r="M46" s="4">
         <v>1</v>
       </c>
-      <c r="N46" s="11">
+      <c r="N46" s="2">
         <v>0</v>
       </c>
       <c r="O46" s="4">
@@ -5308,13 +5297,13 @@
       <c r="G66" s="1">
         <v>0.17</v>
       </c>
-      <c r="I66" s="11" t="s">
+      <c r="I66" s="2" t="s">
         <v>96</v>
       </c>
       <c r="J66" s="4">
         <v>1</v>
       </c>
-      <c r="K66" s="11">
+      <c r="K66" s="2">
         <v>0</v>
       </c>
       <c r="L66" s="6">
@@ -5324,7 +5313,7 @@
       <c r="M66" s="4">
         <v>6</v>
       </c>
-      <c r="N66" s="11">
+      <c r="N66" s="2">
         <v>6</v>
       </c>
       <c r="O66" s="4">
@@ -5633,13 +5622,13 @@
       <c r="G71" s="1">
         <v>0</v>
       </c>
-      <c r="I71" s="11" t="s">
+      <c r="I71" s="2" t="s">
         <v>104</v>
       </c>
       <c r="J71" s="4">
         <v>0</v>
       </c>
-      <c r="K71" s="11">
+      <c r="K71" s="2">
         <v>1</v>
       </c>
       <c r="L71" s="6">
@@ -5649,7 +5638,7 @@
       <c r="M71" s="4">
         <v>11</v>
       </c>
-      <c r="N71" s="11">
+      <c r="N71" s="2">
         <v>9</v>
       </c>
       <c r="O71" s="4">
@@ -6413,30 +6402,30 @@
       <c r="G83" s="1">
         <v>1</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I83" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="J83" s="4">
+      <c r="J83" s="12">
         <f>SUM(J2:J82)</f>
         <v>667</v>
       </c>
-      <c r="K83" s="4">
+      <c r="K83" s="12">
         <f>SUM(K2:K82)</f>
         <v>542</v>
       </c>
-      <c r="L83" s="6">
+      <c r="L83" s="13">
         <f>Table1[[#This Row],[Actual-Virgin]]-Table1[[#This Row],[Exp-Virgin]]</f>
         <v>-125</v>
       </c>
-      <c r="M83" s="4">
+      <c r="M83" s="12">
         <f>SUM(M2:M82)</f>
         <v>124</v>
       </c>
-      <c r="N83" s="4">
+      <c r="N83" s="12">
         <f>SUM(N2:N82)</f>
         <v>145</v>
       </c>
-      <c r="O83" s="4">
+      <c r="O83" s="12">
         <f>Table1[[#This Row],[Actual-Repro]]-Table1[[#This Row],[Exp-Repro]]</f>
         <v>21</v>
       </c>
@@ -8900,22 +8889,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
@@ -8926,12 +8899,28 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:G1048576">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$C1="Virgin"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$C1="REPROCESS"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>